<commit_message>
ajout script mise en forme + unmarked
</commit_message>
<xml_diff>
--- a/Dataset/marmottes2025_renamedMB.xlsx
+++ b/Dataset/marmottes2025_renamedMB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FDC_Savoie\Marmottes_Savoie_2025\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7906B5-D00A-4319-A603-FE1632B60D02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B6A4F1-B7C4-40E2-81EC-8CE5FB9996EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025_Marmotte_Base_de_Donnees" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5677" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5677" uniqueCount="196">
   <si>
     <t>date</t>
   </si>
@@ -632,6 +632,9 @@
   </si>
   <si>
     <t>individu</t>
+  </si>
+  <si>
+    <t>secteur</t>
   </si>
 </sst>
 </file>
@@ -1225,9 +1228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O553"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="30" customHeight="1"/>
   <cols>
@@ -1250,7 +1251,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="30" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>179</v>
@@ -27112,7 +27113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC903D6C-3B1E-4A55-9A38-8B7FEC304466}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>